<commit_message>
cube sizes and cut places
git-svn-id: http://www.ardentheavyindustries.com/svn/syzygryd/trunk@409 1c6c7da2-4a7c-0410-9345-fc53533f7dce
</commit_message>
<xml_diff>
--- a/cad/Solidworks Assemblies/cubes/cube_sizes.xlsx
+++ b/cad/Solidworks Assemblies/cubes/cube_sizes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>cube01</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>meters</t>
+  </si>
+  <si>
+    <t>Gap</t>
+  </si>
+  <si>
+    <t>StripWidth</t>
   </si>
 </sst>
 </file>
@@ -505,15 +511,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="90.75">
+    <row r="1" spans="1:11" ht="90.75">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>36</v>
@@ -530,8 +536,14 @@
       <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +566,18 @@
         <f>E2*2.24/10</f>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2">
+        <f>ROUND(B2,1) - ($J$2 + $K$2 + 0.14) * 2</f>
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="J2">
+        <v>0.375</v>
+      </c>
+      <c r="K2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,8 +600,12 @@
         <f t="shared" ref="F3:F37" si="3">E3*2.24/10</f>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <f t="shared" ref="H3:H37" si="4">ROUND(B3,1) - ($J$2 + $K$2 + 0.14) * 2</f>
+        <v>3.8199999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -602,8 +628,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>3.5199999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -626,8 +656,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -650,8 +684,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -675,7 +713,7 @@
         <v>1.7920000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:11">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -699,7 +737,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:11">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -723,7 +761,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:11">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -747,7 +785,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:11">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -771,7 +809,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:11">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -795,7 +833,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:11">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -819,7 +857,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:11">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -843,7 +881,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:11">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -867,7 +905,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:11">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -891,7 +929,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -915,7 +953,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -939,7 +977,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -963,7 +1001,7 @@
         <v>0.89600000000000013</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -987,7 +1025,7 @@
         <v>1.7920000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1010,8 +1048,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1034,8 +1076,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1058,8 +1104,12 @@
         <f t="shared" si="3"/>
         <v>2.6880000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>7.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1082,8 +1132,12 @@
         <f t="shared" si="3"/>
         <v>3.5840000000000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>10.32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1106,8 +1160,12 @@
         <f t="shared" si="3"/>
         <v>3.5840000000000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>13.219999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1130,8 +1188,12 @@
         <f t="shared" si="3"/>
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>16.22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1154,8 +1216,12 @@
         <f t="shared" si="3"/>
         <v>5.3760000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>19.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1178,8 +1244,12 @@
         <f t="shared" si="3"/>
         <v>6.2720000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>22.119999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1202,8 +1272,12 @@
         <f t="shared" si="3"/>
         <v>6.2720000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>23.619999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1226,8 +1300,12 @@
         <f t="shared" si="3"/>
         <v>6.2720000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>25.72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1250,8 +1328,12 @@
         <f t="shared" si="3"/>
         <v>7.168000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>27.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1274,8 +1356,12 @@
         <f t="shared" si="3"/>
         <v>7.168000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>27.919999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1298,8 +1384,12 @@
         <f t="shared" si="3"/>
         <v>5.3760000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>17.82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1322,8 +1412,12 @@
         <f t="shared" si="3"/>
         <v>3.5840000000000005</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1346,8 +1440,12 @@
         <f t="shared" si="3"/>
         <v>2.6880000000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>8.620000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1370,8 +1468,12 @@
         <f t="shared" si="3"/>
         <v>2.6880000000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1394,8 +1496,12 @@
         <f t="shared" si="3"/>
         <v>1.7920000000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="F39">
         <f>SUM(F2:F37)</f>
         <v>95.872000000000043</v>

</xml_diff>